<commit_message>
archivo de excel con datos del cliente
</commit_message>
<xml_diff>
--- a/sysvac/admin/TABLA DE VAC.xlsx
+++ b/sysvac/admin/TABLA DE VAC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Luz\02. Nominas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_local\_prog\10_micro\sysvac\admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -306,7 +306,7 @@
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -359,8 +359,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,6 +423,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -445,7 +465,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -534,6 +554,16 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -819,10 +849,10 @@
   <dimension ref="A1:P68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="P10" sqref="P10"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +879,7 @@
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H1" s="23">
         <f ca="1">TODAY()</f>
-        <v>43817</v>
+        <v>43855</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -872,10 +902,10 @@
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="41" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -884,19 +914,19 @@
       <c r="F5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="G5" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H5" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="43" t="s">
         <v>59</v>
       </c>
       <c r="M5" s="29" t="s">
@@ -934,9 +964,9 @@
       </c>
       <c r="G7" s="24">
         <f ca="1">($H$1-C7)/365</f>
-        <v>2.2493150684931509</v>
-      </c>
-      <c r="H7" s="6">
+        <v>2.3534246575342466</v>
+      </c>
+      <c r="H7" s="42">
         <v>6</v>
       </c>
       <c r="I7" s="6">
@@ -980,15 +1010,15 @@
         <v>2000</v>
       </c>
       <c r="E8" s="14">
-        <f t="shared" ref="E8" si="0">D8/7</f>
+        <f>D8/7</f>
         <v>285.71428571428572</v>
       </c>
       <c r="F8" s="12">
         <v>102.68</v>
       </c>
       <c r="G8" s="24">
-        <f t="shared" ref="G8:G35" ca="1" si="1">($H$1-C8)/365</f>
-        <v>2.2876712328767121</v>
+        <f t="shared" ref="G8:G35" ca="1" si="0">($H$1-C8)/365</f>
+        <v>2.3917808219178083</v>
       </c>
       <c r="H8" s="6">
         <v>6</v>
@@ -997,7 +1027,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" ref="J8:J35" si="2">H8-I8</f>
+        <f t="shared" ref="J8:J35" si="1">H8-I8</f>
         <v>0</v>
       </c>
       <c r="K8" s="6" t="s">
@@ -1041,8 +1071,8 @@
         <v>102.68</v>
       </c>
       <c r="G9" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9232876712328768</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0273972602739727</v>
       </c>
       <c r="H9" s="6">
         <v>6</v>
@@ -1089,13 +1119,13 @@
         <v>950</v>
       </c>
       <c r="E10" s="15">
-        <f t="shared" ref="E10:E18" si="3">D10/7</f>
+        <f t="shared" ref="E10:E18" si="2">D10/7</f>
         <v>135.71428571428572</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.3205479452054794</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.4246575342465753</v>
       </c>
       <c r="H10" s="6">
         <v>6</v>
@@ -1104,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K10" s="6" t="s">
@@ -1148,8 +1178,8 @@
         <v>102.68</v>
       </c>
       <c r="G11" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9616438356164383</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0657534246575344</v>
       </c>
       <c r="H11" s="6">
         <v>6</v>
@@ -1158,7 +1188,7 @@
         <v>6</v>
       </c>
       <c r="J11" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K11" s="6" t="s">
@@ -1195,16 +1225,16 @@
         <v>900</v>
       </c>
       <c r="E12" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>128.57142857142858</v>
       </c>
       <c r="F12" s="5"/>
       <c r="G12" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.4054794520547946</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5095890410958903</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1222,15 +1252,15 @@
         <v>1496.71</v>
       </c>
       <c r="E13" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>213.81571428571428</v>
       </c>
       <c r="F13" s="12">
         <v>102.68</v>
       </c>
       <c r="G13" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.7123287671232876</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8164383561643835</v>
       </c>
       <c r="H13" s="6">
         <v>6</v>
@@ -1239,7 +1269,7 @@
         <v>6</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K13" s="23" t="s">
@@ -1276,15 +1306,15 @@
         <v>1250</v>
       </c>
       <c r="E14" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>178.57142857142858</v>
       </c>
       <c r="F14" s="12">
         <v>102.68</v>
       </c>
       <c r="G14" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9232876712328768</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0273972602739727</v>
       </c>
       <c r="H14" s="6">
         <v>6</v>
@@ -1293,7 +1323,7 @@
         <v>6</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K14" s="6" t="s">
@@ -1330,15 +1360,15 @@
         <v>1250</v>
       </c>
       <c r="E15" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>178.57142857142858</v>
       </c>
       <c r="F15" s="12">
         <v>102.68</v>
       </c>
       <c r="G15" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.4438356164383561</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.547945205479452</v>
       </c>
       <c r="H15" s="6">
         <v>6</v>
@@ -1347,7 +1377,7 @@
         <v>3</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K15" s="6" t="s">
@@ -1384,15 +1414,15 @@
         <v>1000</v>
       </c>
       <c r="E16" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>142.85714285714286</v>
       </c>
       <c r="F16" s="12">
         <v>106.68</v>
       </c>
       <c r="G16" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.263013698630137</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.3671232876712329</v>
       </c>
       <c r="H16" s="6">
         <v>6</v>
@@ -1401,7 +1431,7 @@
         <v>2</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K16" s="6" t="s">
@@ -1439,13 +1469,13 @@
         <v>950</v>
       </c>
       <c r="E17" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>135.71428571428572</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.1561643835616437</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2602739726027397</v>
       </c>
       <c r="H17" s="6">
         <v>6</v>
@@ -1491,16 +1521,16 @@
         <v>1250</v>
       </c>
       <c r="E18" s="15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>178.57142857142858</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.1369863013698631</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.2410958904109588</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1523,15 +1553,15 @@
         <v>3452.0547945205481</v>
       </c>
       <c r="E20" s="14">
-        <f t="shared" ref="E20:E30" si="4">D20/7</f>
+        <f t="shared" ref="E20:E30" si="3">D20/7</f>
         <v>493.15068493150687</v>
       </c>
       <c r="F20" s="12">
         <v>102.68</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8630136986301369</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9671232876712328</v>
       </c>
       <c r="H20" s="6">
         <v>6</v>
@@ -1540,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="J20" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K20" s="6" t="s">
@@ -1577,13 +1607,13 @@
         <v>5339.18</v>
       </c>
       <c r="E21" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>762.74</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>2.547945205479452</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.6520547945205482</v>
       </c>
       <c r="H21" s="6">
         <v>8</v>
@@ -1592,7 +1622,7 @@
         <v>4</v>
       </c>
       <c r="J21" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K21" s="6" t="s">
@@ -1629,19 +1659,19 @@
         <v>3500</v>
       </c>
       <c r="E22" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9616438356164383</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0657534246575344</v>
       </c>
       <c r="H22" s="6">
         <v>6</v>
       </c>
       <c r="J22" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1660,19 +1690,19 @@
         <v>3999.9994520547948</v>
       </c>
       <c r="E23" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>571.42849315068497</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9616438356164383</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0657534246575344</v>
       </c>
       <c r="H23" s="6">
         <v>6</v>
       </c>
       <c r="J23" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1691,18 +1721,18 @@
         <v>3452.0547945205481</v>
       </c>
       <c r="E24" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>493.15068493150687</v>
       </c>
       <c r="F24" s="12">
         <v>102.68</v>
       </c>
       <c r="G24" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.4575342465753425</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.5616438356164384</v>
       </c>
       <c r="J24" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
@@ -1721,15 +1751,15 @@
         <v>2761.6438356164381</v>
       </c>
       <c r="E25" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>394.52054794520546</v>
       </c>
       <c r="F25" s="12">
         <v>102.68</v>
       </c>
       <c r="G25" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.8630136986301369</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.9671232876712328</v>
       </c>
       <c r="H25" s="6">
         <v>6</v>
@@ -1739,7 +1769,7 @@
         <v>4</v>
       </c>
       <c r="J25" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K25" s="6" t="s">
@@ -1776,15 +1806,15 @@
         <v>3850</v>
       </c>
       <c r="E26" s="21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>550</v>
       </c>
       <c r="F26" s="12">
         <v>102.68</v>
       </c>
       <c r="G26" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.6109589041095891</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.7150684931506848</v>
       </c>
       <c r="H26" s="6">
         <v>8</v>
@@ -1793,7 +1823,7 @@
         <v>4</v>
       </c>
       <c r="J26" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="K26" s="6" t="s">
@@ -1830,21 +1860,21 @@
         <v>3500</v>
       </c>
       <c r="E27" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>500</v>
       </c>
       <c r="F27" s="12">
         <v>102.68</v>
       </c>
       <c r="G27" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9616438356164383</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0657534246575344</v>
       </c>
       <c r="H27" s="6">
         <v>6</v>
       </c>
       <c r="J27" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="O27" s="32"/>
@@ -1863,15 +1893,15 @@
         <v>6907.9</v>
       </c>
       <c r="E28" s="10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>986.84285714285704</v>
       </c>
       <c r="F28" s="12">
         <v>102.68</v>
       </c>
       <c r="G28" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.1123287671232878</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.2164383561643834</v>
       </c>
       <c r="H28" s="6">
         <v>8</v>
@@ -1880,7 +1910,7 @@
         <v>8</v>
       </c>
       <c r="J28" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K28" s="6" t="s">
@@ -1918,19 +1948,19 @@
         <v>5000.0021917808226</v>
       </c>
       <c r="E29" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>714.28602739726034</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9616438356164383</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0657534246575344</v>
       </c>
       <c r="H29" s="6">
         <v>6</v>
       </c>
       <c r="J29" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1949,19 +1979,19 @@
         <v>3500.0038356164387</v>
       </c>
       <c r="E30" s="15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>500.00054794520554</v>
       </c>
       <c r="F30" s="12"/>
       <c r="G30" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>1.9616438356164383</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.0657534246575344</v>
       </c>
       <c r="H30" s="6">
         <v>6</v>
       </c>
       <c r="J30" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
     </row>
@@ -1992,14 +2022,14 @@
         <v>102.68</v>
       </c>
       <c r="G32" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.9643835616438357</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4.0684931506849313</v>
       </c>
       <c r="H32" s="6">
         <v>10</v>
       </c>
       <c r="J32" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="M32" s="30"/>
@@ -2025,8 +2055,8 @@
         <v>0</v>
       </c>
       <c r="G34" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.21643835616438356</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.32054794520547947</v>
       </c>
       <c r="H34" s="6">
         <v>6</v>
@@ -2035,7 +2065,7 @@
         <v>5</v>
       </c>
       <c r="J34" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K34" s="6" t="s">
@@ -2076,8 +2106,8 @@
         <v>102.68</v>
       </c>
       <c r="G35" s="24">
-        <f t="shared" ca="1" si="1"/>
-        <v>0.67671232876712328</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>0.78082191780821919</v>
       </c>
       <c r="H35" s="6">
         <v>6</v>
@@ -2086,7 +2116,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="K35" s="23">
@@ -2260,6 +2290,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>